<commit_message>
US group 2 reruns
</commit_message>
<xml_diff>
--- a/applications/us_states/Chicago_validation.xlsx
+++ b/applications/us_states/Chicago_validation.xlsx
@@ -465,28 +465,28 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3">
-        <v>37646</v>
+        <v>40901</v>
       </c>
       <c r="B3">
-        <v>40265</v>
+        <v>46627</v>
       </c>
       <c r="C3">
-        <v>42650</v>
+        <v>51326</v>
       </c>
       <c r="D3">
-        <v>53889</v>
+        <v>65202</v>
       </c>
       <c r="I3">
-        <v>1676</v>
+        <v>1594</v>
       </c>
       <c r="J3">
-        <v>1873</v>
+        <v>1775</v>
       </c>
       <c r="K3">
-        <v>2077</v>
+        <v>1910</v>
       </c>
       <c r="L3">
-        <v>2632</v>
+        <v>2347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>